<commit_message>
Added access point to API doc
</commit_message>
<xml_diff>
--- a/docs/Read-Write-API.xlsx
+++ b/docs/Read-Write-API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\mbr01458\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREPO\Linked-Data-Theatre\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="98">
   <si>
     <t>Type</t>
   </si>
@@ -307,6 +307,21 @@
   </si>
   <si>
     <t>Collection replaced</t>
+  </si>
+  <si>
+    <t>Access-point for resources</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>/{access-point}?resource={URI}</t>
+  </si>
+  <si>
+    <t>Access-point for named graphs</t>
+  </si>
+  <si>
+    <t>/{access-point}?graph={URI}</t>
   </si>
 </sst>
 </file>
@@ -936,17 +951,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
@@ -1817,6 +1832,290 @@
         <v>78</v>
       </c>
     </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" t="s">
+        <v>76</v>
+      </c>
+      <c r="H37" t="s">
+        <v>77</v>
+      </c>
+      <c r="I37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" t="s">
+        <v>77</v>
+      </c>
+      <c r="I39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" t="s">
+        <v>77</v>
+      </c>
+      <c r="I43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" t="s">
+        <v>77</v>
+      </c>
+      <c r="I44" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I34"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>